<commit_message>
Create LEEME file with instructions on how to use this folder
</commit_message>
<xml_diff>
--- a/tables/listado_etapas_GES.xlsx
+++ b/tables/listado_etapas_GES.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\auge1\Desktop\Proyectos R\reporte_ges\tables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/13c0fce16975a509/Proyectos R/reporte_GES/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{763783D0-E8DB-47C4-974B-8449776BF6ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{763783D0-E8DB-47C4-974B-8449776BF6ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0603F128-C478-4671-AFCC-00F61B33D061}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{AF8272FD-15FE-46C4-818B-396B93757DD0}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AF8272FD-15FE-46C4-818B-396B93757DD0}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -1396,21 +1396,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CA65C38-E6C2-4E50-92A5-3EAF4572B1D9}">
   <dimension ref="A1:G295"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="90.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="66.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.28515625" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" customWidth="1"/>
-    <col min="5" max="5" width="21.42578125" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" customWidth="1"/>
+    <col min="1" max="1" width="90.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="66.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.33203125" customWidth="1"/>
+    <col min="4" max="4" width="16.109375" customWidth="1"/>
+    <col min="5" max="5" width="21.44140625" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1433,7 +1433,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1456,7 +1456,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1479,7 +1479,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1502,7 +1502,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1525,7 +1525,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -1548,7 +1548,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -1571,7 +1571,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -1594,7 +1594,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -1617,7 +1617,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -1640,7 +1640,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -1663,7 +1663,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -1686,7 +1686,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -1709,7 +1709,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -1732,7 +1732,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -1755,7 +1755,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -1778,7 +1778,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -1801,7 +1801,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>23</v>
       </c>
@@ -1824,7 +1824,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -1847,7 +1847,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -1870,7 +1870,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>27</v>
       </c>
@@ -1893,7 +1893,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>27</v>
       </c>
@@ -1916,7 +1916,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>27</v>
       </c>
@@ -1939,7 +1939,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>31</v>
       </c>
@@ -1962,7 +1962,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>31</v>
       </c>
@@ -1985,7 +1985,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>31</v>
       </c>
@@ -2008,7 +2008,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>31</v>
       </c>
@@ -2031,7 +2031,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>34</v>
       </c>
@@ -2054,7 +2054,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>34</v>
       </c>
@@ -2077,7 +2077,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>34</v>
       </c>
@@ -2100,7 +2100,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>36</v>
       </c>
@@ -2123,7 +2123,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>36</v>
       </c>
@@ -2146,7 +2146,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>36</v>
       </c>
@@ -2169,7 +2169,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>36</v>
       </c>
@@ -2192,7 +2192,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>36</v>
       </c>
@@ -2215,7 +2215,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>36</v>
       </c>
@@ -2238,7 +2238,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -2261,7 +2261,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>36</v>
       </c>
@@ -2284,7 +2284,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>36</v>
       </c>
@@ -2307,7 +2307,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>42</v>
       </c>
@@ -2330,7 +2330,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>42</v>
       </c>
@@ -2353,7 +2353,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>42</v>
       </c>
@@ -2376,7 +2376,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>42</v>
       </c>
@@ -2399,7 +2399,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>42</v>
       </c>
@@ -2422,7 +2422,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>42</v>
       </c>
@@ -2445,7 +2445,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>42</v>
       </c>
@@ -2468,7 +2468,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>42</v>
       </c>
@@ -2491,7 +2491,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>42</v>
       </c>
@@ -2514,7 +2514,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>42</v>
       </c>
@@ -2537,7 +2537,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>42</v>
       </c>
@@ -2560,7 +2560,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>42</v>
       </c>
@@ -2583,7 +2583,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>42</v>
       </c>
@@ -2606,7 +2606,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>55</v>
       </c>
@@ -2629,7 +2629,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>55</v>
       </c>
@@ -2652,7 +2652,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>55</v>
       </c>
@@ -2675,7 +2675,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>55</v>
       </c>
@@ -2698,7 +2698,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>60</v>
       </c>
@@ -2721,7 +2721,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>60</v>
       </c>
@@ -2744,7 +2744,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>63</v>
       </c>
@@ -2767,7 +2767,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>63</v>
       </c>
@@ -2790,7 +2790,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>63</v>
       </c>
@@ -2813,7 +2813,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>67</v>
       </c>
@@ -2836,7 +2836,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>67</v>
       </c>
@@ -2859,7 +2859,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>67</v>
       </c>
@@ -2882,7 +2882,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>67</v>
       </c>
@@ -2905,7 +2905,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>67</v>
       </c>
@@ -2928,7 +2928,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>73</v>
       </c>
@@ -2951,7 +2951,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>75</v>
       </c>
@@ -2974,7 +2974,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>75</v>
       </c>
@@ -2997,7 +2997,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>75</v>
       </c>
@@ -3020,7 +3020,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>75</v>
       </c>
@@ -3043,7 +3043,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>75</v>
       </c>
@@ -3066,7 +3066,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>75</v>
       </c>
@@ -3089,7 +3089,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>75</v>
       </c>
@@ -3112,7 +3112,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>75</v>
       </c>
@@ -3135,7 +3135,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>83</v>
       </c>
@@ -3158,7 +3158,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>83</v>
       </c>
@@ -3181,7 +3181,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>83</v>
       </c>
@@ -3204,7 +3204,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>83</v>
       </c>
@@ -3227,7 +3227,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>83</v>
       </c>
@@ -3250,7 +3250,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>83</v>
       </c>
@@ -3273,7 +3273,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>83</v>
       </c>
@@ -3296,7 +3296,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>83</v>
       </c>
@@ -3319,7 +3319,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>92</v>
       </c>
@@ -3342,7 +3342,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>92</v>
       </c>
@@ -3365,7 +3365,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>92</v>
       </c>
@@ -3388,7 +3388,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>92</v>
       </c>
@@ -3411,7 +3411,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>95</v>
       </c>
@@ -3434,7 +3434,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>95</v>
       </c>
@@ -3457,7 +3457,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>95</v>
       </c>
@@ -3480,7 +3480,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>95</v>
       </c>
@@ -3503,7 +3503,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>95</v>
       </c>
@@ -3526,7 +3526,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>97</v>
       </c>
@@ -3549,7 +3549,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>97</v>
       </c>
@@ -3572,7 +3572,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>97</v>
       </c>
@@ -3595,7 +3595,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>98</v>
       </c>
@@ -3618,7 +3618,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>98</v>
       </c>
@@ -3641,7 +3641,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>101</v>
       </c>
@@ -3664,7 +3664,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>102</v>
       </c>
@@ -3687,7 +3687,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>102</v>
       </c>
@@ -3710,7 +3710,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>102</v>
       </c>
@@ -3733,7 +3733,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>106</v>
       </c>
@@ -3756,7 +3756,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>106</v>
       </c>
@@ -3779,7 +3779,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>106</v>
       </c>
@@ -3802,7 +3802,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>106</v>
       </c>
@@ -3825,7 +3825,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>111</v>
       </c>
@@ -3848,7 +3848,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>111</v>
       </c>
@@ -3871,7 +3871,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>111</v>
       </c>
@@ -3894,7 +3894,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>111</v>
       </c>
@@ -3917,7 +3917,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>111</v>
       </c>
@@ -3940,7 +3940,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>115</v>
       </c>
@@ -3963,7 +3963,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>117</v>
       </c>
@@ -3986,7 +3986,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>119</v>
       </c>
@@ -4009,7 +4009,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>119</v>
       </c>
@@ -4032,7 +4032,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>119</v>
       </c>
@@ -4055,7 +4055,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>119</v>
       </c>
@@ -4078,7 +4078,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>122</v>
       </c>
@@ -4101,7 +4101,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>122</v>
       </c>
@@ -4124,7 +4124,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>123</v>
       </c>
@@ -4147,7 +4147,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>123</v>
       </c>
@@ -4170,7 +4170,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>123</v>
       </c>
@@ -4193,7 +4193,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>124</v>
       </c>
@@ -4216,7 +4216,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>124</v>
       </c>
@@ -4239,7 +4239,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>127</v>
       </c>
@@ -4262,7 +4262,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>127</v>
       </c>
@@ -4285,7 +4285,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>130</v>
       </c>
@@ -4308,7 +4308,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>130</v>
       </c>
@@ -4331,7 +4331,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>130</v>
       </c>
@@ -4354,7 +4354,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>134</v>
       </c>
@@ -4377,7 +4377,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>135</v>
       </c>
@@ -4400,7 +4400,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>137</v>
       </c>
@@ -4423,7 +4423,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>137</v>
       </c>
@@ -4446,7 +4446,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>140</v>
       </c>
@@ -4469,7 +4469,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>140</v>
       </c>
@@ -4492,7 +4492,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>140</v>
       </c>
@@ -4515,7 +4515,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>140</v>
       </c>
@@ -4538,7 +4538,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>140</v>
       </c>
@@ -4561,7 +4561,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>140</v>
       </c>
@@ -4584,7 +4584,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>140</v>
       </c>
@@ -4607,7 +4607,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>140</v>
       </c>
@@ -4630,7 +4630,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>147</v>
       </c>
@@ -4653,7 +4653,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>147</v>
       </c>
@@ -4676,7 +4676,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>147</v>
       </c>
@@ -4699,7 +4699,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>147</v>
       </c>
@@ -4722,7 +4722,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>147</v>
       </c>
@@ -4745,7 +4745,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>150</v>
       </c>
@@ -4768,7 +4768,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>150</v>
       </c>
@@ -4791,7 +4791,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>150</v>
       </c>
@@ -4814,7 +4814,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>150</v>
       </c>
@@ -4837,7 +4837,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>150</v>
       </c>
@@ -4860,7 +4860,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>153</v>
       </c>
@@ -4883,7 +4883,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>154</v>
       </c>
@@ -4906,7 +4906,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>154</v>
       </c>
@@ -4929,7 +4929,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>155</v>
       </c>
@@ -4952,7 +4952,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>156</v>
       </c>
@@ -4975,7 +4975,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>156</v>
       </c>
@@ -4998,7 +4998,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>156</v>
       </c>
@@ -5021,7 +5021,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>160</v>
       </c>
@@ -5044,7 +5044,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>161</v>
       </c>
@@ -5067,7 +5067,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>161</v>
       </c>
@@ -5090,7 +5090,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>164</v>
       </c>
@@ -5113,7 +5113,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>166</v>
       </c>
@@ -5136,7 +5136,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>166</v>
       </c>
@@ -5159,7 +5159,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>168</v>
       </c>
@@ -5182,7 +5182,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>168</v>
       </c>
@@ -5205,7 +5205,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>170</v>
       </c>
@@ -5228,7 +5228,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>170</v>
       </c>
@@ -5251,7 +5251,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>171</v>
       </c>
@@ -5274,7 +5274,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>171</v>
       </c>
@@ -5297,7 +5297,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>171</v>
       </c>
@@ -5320,7 +5320,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>173</v>
       </c>
@@ -5343,7 +5343,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>175</v>
       </c>
@@ -5366,7 +5366,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>177</v>
       </c>
@@ -5389,7 +5389,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>177</v>
       </c>
@@ -5412,7 +5412,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>177</v>
       </c>
@@ -5435,7 +5435,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>177</v>
       </c>
@@ -5458,7 +5458,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="177" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>177</v>
       </c>
@@ -5481,7 +5481,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="178" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>178</v>
       </c>
@@ -5504,7 +5504,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>178</v>
       </c>
@@ -5527,7 +5527,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="180" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>178</v>
       </c>
@@ -5550,7 +5550,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>179</v>
       </c>
@@ -5573,7 +5573,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>179</v>
       </c>
@@ -5596,7 +5596,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>179</v>
       </c>
@@ -5619,7 +5619,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>179</v>
       </c>
@@ -5642,7 +5642,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>179</v>
       </c>
@@ -5665,7 +5665,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="186" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>179</v>
       </c>
@@ -5688,7 +5688,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="187" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>179</v>
       </c>
@@ -5711,7 +5711,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="188" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>187</v>
       </c>
@@ -5734,7 +5734,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="189" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>187</v>
       </c>
@@ -5757,7 +5757,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="190" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
         <v>189</v>
       </c>
@@ -5780,7 +5780,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="191" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>189</v>
       </c>
@@ -5803,7 +5803,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="192" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
         <v>191</v>
       </c>
@@ -5826,7 +5826,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="193" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>191</v>
       </c>
@@ -5849,7 +5849,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="194" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>192</v>
       </c>
@@ -5872,7 +5872,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="195" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>192</v>
       </c>
@@ -5895,7 +5895,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="196" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>192</v>
       </c>
@@ -5918,7 +5918,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="197" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>193</v>
       </c>
@@ -5941,7 +5941,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="198" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
         <v>193</v>
       </c>
@@ -5964,7 +5964,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="199" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>193</v>
       </c>
@@ -5987,7 +5987,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="200" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>193</v>
       </c>
@@ -6010,7 +6010,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="201" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>196</v>
       </c>
@@ -6033,7 +6033,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="202" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
         <v>197</v>
       </c>
@@ -6056,7 +6056,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="203" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
         <v>198</v>
       </c>
@@ -6079,7 +6079,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="204" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
         <v>198</v>
       </c>
@@ -6102,7 +6102,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="205" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
         <v>200</v>
       </c>
@@ -6125,7 +6125,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="206" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
         <v>202</v>
       </c>
@@ -6148,7 +6148,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="207" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
         <v>202</v>
       </c>
@@ -6171,7 +6171,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="208" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
         <v>202</v>
       </c>
@@ -6194,7 +6194,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="209" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
         <v>205</v>
       </c>
@@ -6217,7 +6217,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="210" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
         <v>205</v>
       </c>
@@ -6240,7 +6240,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="211" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
         <v>205</v>
       </c>
@@ -6263,7 +6263,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="212" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
         <v>205</v>
       </c>
@@ -6286,7 +6286,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="213" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
         <v>206</v>
       </c>
@@ -6309,7 +6309,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="214" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
         <v>206</v>
       </c>
@@ -6332,7 +6332,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="215" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
         <v>206</v>
       </c>
@@ -6355,7 +6355,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="216" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
         <v>208</v>
       </c>
@@ -6378,7 +6378,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="217" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
         <v>208</v>
       </c>
@@ -6401,7 +6401,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="218" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
         <v>210</v>
       </c>
@@ -6424,7 +6424,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="219" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
         <v>210</v>
       </c>
@@ -6447,7 +6447,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="220" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
         <v>210</v>
       </c>
@@ -6470,7 +6470,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="221" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
         <v>210</v>
       </c>
@@ -6493,7 +6493,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="222" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
         <v>213</v>
       </c>
@@ -6516,7 +6516,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="223" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
         <v>215</v>
       </c>
@@ -6539,7 +6539,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="224" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
         <v>216</v>
       </c>
@@ -6562,7 +6562,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="225" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
         <v>217</v>
       </c>
@@ -6585,7 +6585,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="226" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
         <v>217</v>
       </c>
@@ -6608,7 +6608,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="227" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
         <v>217</v>
       </c>
@@ -6631,7 +6631,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="228" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
         <v>219</v>
       </c>
@@ -6654,7 +6654,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="229" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
         <v>219</v>
       </c>
@@ -6677,7 +6677,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="230" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
         <v>219</v>
       </c>
@@ -6700,7 +6700,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="231" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
         <v>223</v>
       </c>
@@ -6723,7 +6723,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="232" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
         <v>225</v>
       </c>
@@ -6746,7 +6746,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="233" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
         <v>227</v>
       </c>
@@ -6769,7 +6769,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="234" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
         <v>227</v>
       </c>
@@ -6792,7 +6792,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="235" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
         <v>230</v>
       </c>
@@ -6815,7 +6815,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="236" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
         <v>230</v>
       </c>
@@ -6838,7 +6838,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="237" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
         <v>230</v>
       </c>
@@ -6861,7 +6861,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="238" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
         <v>234</v>
       </c>
@@ -6884,7 +6884,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="239" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
         <v>234</v>
       </c>
@@ -6907,7 +6907,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="240" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
         <v>234</v>
       </c>
@@ -6930,7 +6930,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="241" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
         <v>237</v>
       </c>
@@ -6953,7 +6953,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="242" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
         <v>239</v>
       </c>
@@ -6976,7 +6976,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="243" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
         <v>239</v>
       </c>
@@ -6999,7 +6999,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="244" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
         <v>335</v>
       </c>
@@ -7022,7 +7022,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="245" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
         <v>240</v>
       </c>
@@ -7045,7 +7045,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="246" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
         <v>240</v>
       </c>
@@ -7068,7 +7068,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="247" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
         <v>241</v>
       </c>
@@ -7091,7 +7091,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="248" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
         <v>241</v>
       </c>
@@ -7114,7 +7114,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="249" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
         <v>242</v>
       </c>
@@ -7137,7 +7137,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="250" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
         <v>242</v>
       </c>
@@ -7160,7 +7160,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="251" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
         <v>245</v>
       </c>
@@ -7183,7 +7183,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="252" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
         <v>247</v>
       </c>
@@ -7206,7 +7206,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="253" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
         <v>249</v>
       </c>
@@ -7229,7 +7229,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="254" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
         <v>249</v>
       </c>
@@ -7252,7 +7252,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="255" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
         <v>252</v>
       </c>
@@ -7275,7 +7275,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="256" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
         <v>254</v>
       </c>
@@ -7298,7 +7298,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="257" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
         <v>254</v>
       </c>
@@ -7321,7 +7321,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="258" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
         <v>254</v>
       </c>
@@ -7344,7 +7344,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="259" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
         <v>258</v>
       </c>
@@ -7367,7 +7367,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="260" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
         <v>260</v>
       </c>
@@ -7390,7 +7390,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="261" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
         <v>260</v>
       </c>
@@ -7413,7 +7413,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="262" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
         <v>261</v>
       </c>
@@ -7436,7 +7436,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="263" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
         <v>261</v>
       </c>
@@ -7459,7 +7459,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="264" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A264" t="s">
         <v>261</v>
       </c>
@@ -7482,7 +7482,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="265" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
         <v>261</v>
       </c>
@@ -7505,7 +7505,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="266" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A266" t="s">
         <v>263</v>
       </c>
@@ -7528,7 +7528,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="267" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
         <v>264</v>
       </c>
@@ -7551,7 +7551,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="268" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A268" t="s">
         <v>266</v>
       </c>
@@ -7574,7 +7574,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="269" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A269" t="s">
         <v>266</v>
       </c>
@@ -7597,7 +7597,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="270" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A270" t="s">
         <v>269</v>
       </c>
@@ -7620,7 +7620,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="271" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
         <v>271</v>
       </c>
@@ -7643,7 +7643,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="272" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
         <v>272</v>
       </c>
@@ -7666,7 +7666,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="273" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
         <v>272</v>
       </c>
@@ -7689,7 +7689,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="274" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A274" t="s">
         <v>273</v>
       </c>
@@ -7712,7 +7712,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="275" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A275" t="s">
         <v>274</v>
       </c>
@@ -7735,7 +7735,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="276" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A276" t="s">
         <v>274</v>
       </c>
@@ -7758,7 +7758,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="277" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A277" t="s">
         <v>275</v>
       </c>
@@ -7781,7 +7781,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="278" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A278" t="s">
         <v>275</v>
       </c>
@@ -7804,7 +7804,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="279" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A279" t="s">
         <v>276</v>
       </c>
@@ -7827,7 +7827,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="280" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A280" t="s">
         <v>276</v>
       </c>
@@ -7850,7 +7850,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="281" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
         <v>277</v>
       </c>
@@ -7873,7 +7873,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="282" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A282" t="s">
         <v>277</v>
       </c>
@@ -7896,7 +7896,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="283" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A283" t="s">
         <v>278</v>
       </c>
@@ -7919,7 +7919,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="284" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A284" t="s">
         <v>278</v>
       </c>
@@ -7942,7 +7942,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="285" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A285" t="s">
         <v>279</v>
       </c>
@@ -7965,7 +7965,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="286" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A286" t="s">
         <v>279</v>
       </c>
@@ -7988,7 +7988,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="287" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A287" t="s">
         <v>280</v>
       </c>
@@ -8011,7 +8011,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="288" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A288" t="s">
         <v>282</v>
       </c>
@@ -8034,7 +8034,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="289" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A289" t="s">
         <v>284</v>
       </c>
@@ -8057,7 +8057,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="290" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A290" t="s">
         <v>285</v>
       </c>
@@ -8080,7 +8080,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="291" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A291" t="s">
         <v>285</v>
       </c>
@@ -8103,7 +8103,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="292" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A292" t="s">
         <v>285</v>
       </c>
@@ -8126,7 +8126,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="293" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A293" t="s">
         <v>285</v>
       </c>
@@ -8149,7 +8149,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="294" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A294" t="s">
         <v>285</v>
       </c>
@@ -8172,7 +8172,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="295" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A295" t="s">
         <v>285</v>
       </c>

</xml_diff>